<commit_message>
Certificat SSL skipped End of the first question Begining of the second question
</commit_message>
<xml_diff>
--- a/Deuxième Dataset Tour1.xlsx
+++ b/Deuxième Dataset Tour1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,40 +535,6 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Camillo_Francesco_Maria_Pamphili</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/1622</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Naples</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Benjamin_Hoadly</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/1676</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Kent</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
finisk new interface for page two. Add proposition to df resultat
</commit_message>
<xml_diff>
--- a/Deuxième Dataset Tour1.xlsx
+++ b/Deuxième Dataset Tour1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,57 +484,6 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Charles_Januarius_Acton</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/1803</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Naples</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Carlo_Barberini</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/1630</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Rome</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Cardinal_de_Bouillon</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/1643</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/France</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected Q2 Done Q3 Done DF resultat filled Done Choice 2
</commit_message>
<xml_diff>
--- a/Deuxième Dataset Tour1.xlsx
+++ b/Deuxième Dataset Tour1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,38 +449,137 @@
           <t>http://dbpedia.org/ontology/birthPlace</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/party</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Dick_Sheppard_(priest)</t>
+          <t>http://dbpedia.org/resource/Barack_Obama</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1880</t>
+          <t>http://dbpedia.org/resource/1961</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Windsor</t>
+          <t>http://dbpedia.org/resource/Honolulu</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Democratic_Party_(United_States)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Claus_Westermann</t>
+          <t>http://dbpedia.org/resource/Benjamin_Harrison</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1909</t>
+          <t>http://dbpedia.org/resource/1833</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Berlin</t>
+          <t>http://dbpedia.org/resource/North_Bend,_Ohio</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Republican_Party_(United_States)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Calvin_Coolidge</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1872</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Plymouth_Notch,_Vermont</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Republican_Party_(United_States)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Harry_S._Truman</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1884</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Lamar</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Missouri</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Herbert_Hoover</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1874</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Iowa</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Lyndon_B._Johnson</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1908</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Stonewall</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Texas</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Rafraichissement des frames apres un nème uri_load
</commit_message>
<xml_diff>
--- a/Deuxième Dataset Tour1.xlsx
+++ b/Deuxième Dataset Tour1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,123 +449,137 @@
           <t>http://dbpedia.org/ontology/birthPlace</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/party</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Dick_Sheppard_(priest)</t>
+          <t>http://dbpedia.org/resource/Barack_Obama</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1880</t>
+          <t>http://dbpedia.org/resource/1961</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Windsor</t>
+          <t>http://dbpedia.org/resource/Honolulu</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Democratic_Party_(United_States)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Claus_Westermann</t>
+          <t>http://dbpedia.org/resource/Benjamin_Harrison</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1909</t>
+          <t>http://dbpedia.org/resource/1833</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Berlin</t>
+          <t>http://dbpedia.org/resource/North_Bend,_Ohio</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Republican_Party_(United_States)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Charles_Januarius_Acton</t>
+          <t>http://dbpedia.org/resource/Calvin_Coolidge</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1803</t>
+          <t>http://dbpedia.org/resource/1872</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Naples</t>
+          <t>http://dbpedia.org/resource/Plymouth_Notch,_Vermont</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Republican_Party_(United_States)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Carlo_Barberini</t>
+          <t>http://dbpedia.org/resource/Harry_S._Truman</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1630</t>
+          <t>http://dbpedia.org/resource/1884</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Rome</t>
+          <t>http://dbpedia.org/resource/Lamar</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Missouri</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Cardinal_de_Bouillon</t>
+          <t>http://dbpedia.org/resource/Herbert_Hoover</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1643</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/France</t>
+          <t>http://dbpedia.org/resource/1874</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Iowa</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Camillo_Francesco_Maria_Pamphili</t>
+          <t>http://dbpedia.org/resource/Lyndon_B._Johnson</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/1622</t>
+          <t>http://dbpedia.org/resource/1908</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Naples</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Benjamin_Hoadly</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/1676</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Kent</t>
+          <t>http://dbpedia.org/resource/Stonewall</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Texas</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor and clean code, pageOne and pageTwo OK pageThree: begin
</commit_message>
<xml_diff>
--- a/Deuxième Dataset Tour1.xlsx
+++ b/Deuxième Dataset Tour1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,65 +441,48 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/championships</t>
+          <t>http://dbpedia.org/ontology/birthDate</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/birthPlace</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Blues_(Breakout_album)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>http://dbpedia.org/resource/Dick_Sheppard_(priest)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1880</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Windsor</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Interview</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Golda_Meir_(Goldfine)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Bill_Self</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Carmine_(color)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Chester_(TTC)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Bill_Self</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+          <t>http://dbpedia.org/resource/Claus_Westermann</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1909</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Berlin</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>